<commit_message>
Figures and Species Info
</commit_message>
<xml_diff>
--- a/NSR_RL/Genome Data/NSR Species Info.xlsx
+++ b/NSR_RL/Genome Data/NSR Species Info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/BDavid/Documents/GitHub/OligoRL/NSR_RL/Genome Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{47F14E3D-44F8-6A42-8275-3998C98575F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BB88C9-18D9-784B-8932-A02704CE2C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38480" yWindow="-2680" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="-9380" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="87">
   <si>
     <t>Download?</t>
   </si>
@@ -278,6 +278,9 @@
   </si>
   <si>
     <t>NC_007604.1, NC_007595.1</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -1128,7 +1131,9 @@
   </sheetPr>
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:H27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1137,7 +1142,7 @@
     <col min="8" max="8" width="40.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1163,7 +1168,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="14" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -1189,7 +1194,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="14" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -1215,7 +1220,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="14" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -1241,7 +1246,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="14" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -1267,7 +1272,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="14" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -1293,7 +1298,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="14" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -1319,7 +1324,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="14" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -1345,7 +1350,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="14" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -1371,7 +1376,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="14" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
@@ -1397,7 +1402,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="14" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
@@ -1423,7 +1428,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="14" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
@@ -1449,7 +1454,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="14" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
@@ -1475,7 +1480,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="14" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>8</v>
       </c>
@@ -1501,9 +1506,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="14" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="B15" s="3">
         <v>14</v>
@@ -1527,7 +1532,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="14" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>8</v>
       </c>
@@ -1553,7 +1558,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="14" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>8</v>
       </c>
@@ -1579,7 +1584,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="14" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>8</v>
       </c>
@@ -1605,7 +1610,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" ht="14" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>8</v>
       </c>
@@ -1631,7 +1636,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="14" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>8</v>
       </c>
@@ -1657,7 +1662,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="14" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>8</v>
       </c>
@@ -1683,7 +1688,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="14" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>8</v>
       </c>
@@ -1709,7 +1714,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="14" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>8</v>
       </c>
@@ -1735,7 +1740,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="14" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>8</v>
       </c>
@@ -1761,7 +1766,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="14" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>8</v>
       </c>
@@ -1787,7 +1792,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="14" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>8</v>
       </c>
@@ -1813,7 +1818,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" ht="14" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>8</v>
       </c>

</xml_diff>